<commit_message>
Fixed minor changes and added more tests.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
+++ b/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DBEDC27B-E902-4CE4-85FC-17F956585F37}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B9DC918A-823B-4E28-BD8B-B1872CD67C73}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22416" windowHeight="10476" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22416" windowHeight="10476" activeTab="2" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RowItems" sheetId="2" r:id="rId2"/>
+    <sheet name="NoSubtotals" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId2"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="29">
   <si>
     <t>Transaction</t>
   </si>
@@ -113,6 +115,9 @@
   <si>
     <t>Headlamp Total</t>
   </si>
+  <si>
+    <t>Sum of Total</t>
+  </si>
 </sst>
 </file>
 
@@ -187,7 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -198,6 +203,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -346,7 +357,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B12:R23" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -499,6 +510,660 @@
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
       <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="L1:M17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="3"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="16">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="PivotTable8" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A26:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFAEB085-386F-48FB-A474-9148F594B553}" name="PivotTable7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="L26:M50" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="3"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="24">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{05E1164D-0C34-4664-8642-A36BC4D23090}" name="PivotTable6" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F26:G38" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:I13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -803,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86234C7-1633-473D-AAFD-744E7802C65D}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1361,4 +2026,828 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEE10A1-DD89-4A58-A7F1-15A3571BC993}">
+  <dimension ref="A1:M50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:B35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="4">
+        <v>2078.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1293</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="4">
+        <v>2078.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4">
+        <v>856.49</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1293</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4228.24</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4">
+        <v>99</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1194</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="4">
+        <v>856.49</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="4">
+        <v>4228.24</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="4">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="4">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="F27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="L27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="F29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M29" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="4">
+        <v>99</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="L30" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M30" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1194</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="4">
+        <v>99</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="F32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="4">
+        <v>1194</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M32" s="4">
+        <v>2078.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="4">
+        <v>1293</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" s="4">
+        <v>2078.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="L34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M34" s="4"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="4">
+        <v>4228.24</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M35" s="4"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F36" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="4">
+        <v>856.49</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="4">
+        <v>4228.24</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M38" s="4"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L39" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M39" s="4">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L40" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M40" s="4">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M41" s="4">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L42" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M42" s="4"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L44" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M44" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L45" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M45" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L46" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M46" s="4"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L47" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M47" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L48" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M48" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="49" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L49" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M49" s="4">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="50" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M50" s="4">
+        <v>4228.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928B7D07-B8BA-40F3-9401-5FCD36095001}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="33" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4">
+        <v>1247.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4">
+        <v>99</v>
+      </c>
+      <c r="I10" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4">
+        <v>199</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="C13" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="D13" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="E13" s="4">
+        <v>199</v>
+      </c>
+      <c r="F13" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="G13" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H13" s="4">
+        <v>99</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1985.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed refreshing pivot table data values in worksheet.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
+++ b/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B9DC918A-823B-4E28-BD8B-B1872CD67C73}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F13B17B0-3153-4F74-AAD2-928BC725C466}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22416" windowHeight="10476" activeTab="2" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22416" windowHeight="10476" activeTab="3" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="RowItems" sheetId="2" r:id="rId2"/>
     <sheet name="NoSubtotals" sheetId="3" r:id="rId3"/>
+    <sheet name="GrandTotals" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="24" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="29">
   <si>
     <t>Transaction</t>
   </si>
@@ -357,7 +358,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B12:R23" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -516,7 +517,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -570,7 +571,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L1:M17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -677,7 +678,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="PivotTable8" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A26:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -753,7 +754,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -831,225 +832,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFAEB085-386F-48FB-A474-9148F594B553}" name="PivotTable7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="L26:M50" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="2"/>
-    <field x="3"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="24">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="3"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{05E1164D-0C34-4664-8642-A36BC4D23090}" name="PivotTable6" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F26:G38" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="12">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:I13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -1164,6 +947,117 @@
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
       <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:L8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -1468,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86234C7-1633-473D-AAFD-744E7802C65D}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:G18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2030,10 +1924,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEE10A1-DD89-4A58-A7F1-15A3571BC993}">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:B35"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2282,36 +2176,16 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="4"/>
-      <c r="F27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="4"/>
-      <c r="L27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M27" s="4"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
@@ -2320,34 +2194,12 @@
       <c r="B28" s="4">
         <v>2078.75</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="4">
-        <v>2078.75</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M28" s="4"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B29" s="4"/>
-      <c r="F29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G29" s="4">
-        <v>2078.75</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="M29" s="4">
-        <v>831.5</v>
-      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
@@ -2356,16 +2208,6 @@
       <c r="B30" s="4">
         <v>99</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="4"/>
-      <c r="L30" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M30" s="4">
-        <v>831.5</v>
-      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
@@ -2374,218 +2216,34 @@
       <c r="B31" s="4">
         <v>1194</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="4">
-        <v>99</v>
-      </c>
-      <c r="L31" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M31" s="4">
-        <v>415.75</v>
-      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="F32" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="4">
-        <v>1194</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M32" s="4">
-        <v>2078.75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B33" s="4">
         <v>831.5</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="4">
-        <v>1293</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M33" s="4">
-        <v>2078.75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B34" s="4">
         <v>24.99</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="4"/>
-      <c r="L34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M34" s="4"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="4">
-        <v>4228.24</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="4">
-        <v>831.5</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M35" s="4"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F36" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="4">
-        <v>24.99</v>
-      </c>
-      <c r="L36" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M36" s="4">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F37" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="4">
-        <v>856.49</v>
-      </c>
-      <c r="L37" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M37" s="4">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F38" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G38" s="4">
-        <v>4228.24</v>
-      </c>
-      <c r="L38" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M38" s="4"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L39" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M39" s="4">
-        <v>1194</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L40" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M40" s="4">
-        <v>1194</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M41" s="4">
-        <v>1293</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L42" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M42" s="4"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L43" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M43" s="4"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L44" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M44" s="4">
-        <v>831.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L45" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M45" s="4">
-        <v>831.5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L46" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M46" s="4"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L47" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="M47" s="4">
-        <v>24.99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L48" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M48" s="4">
-        <v>24.99</v>
-      </c>
-    </row>
-    <row r="49" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L49" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M49" s="4">
-        <v>856.49</v>
-      </c>
-    </row>
-    <row r="50" spans="12:13" x14ac:dyDescent="0.3">
-      <c r="L50" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M50" s="4">
         <v>4228.24</v>
       </c>
     </row>
@@ -2598,17 +2256,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928B7D07-B8BA-40F3-9401-5FCD36095001}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
@@ -2850,4 +2508,222 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2B0220-1F7B-4702-A332-D90617B220D1}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="K4" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="L4" s="4">
+        <v>2910.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="L5" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4">
+        <v>99</v>
+      </c>
+      <c r="H6" s="4">
+        <v>99</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4">
+        <v>1194</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4">
+        <v>1194</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1194</v>
+      </c>
+      <c r="G8" s="4">
+        <v>99</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1293</v>
+      </c>
+      <c r="I8" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="J8" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="K8" s="4">
+        <v>856.49</v>
+      </c>
+      <c r="L8" s="4">
+        <v>4228.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refresh pivot tables that have multiple data fields in the columns.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
+++ b/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F13B17B0-3153-4F74-AAD2-928BC725C466}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{29B48D6B-EB98-4495-86AA-5E6829495C1A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22416" windowHeight="10476" activeTab="3" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22416" windowHeight="10476" activeTab="4" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="RowItems" sheetId="2" r:id="rId2"/>
     <sheet name="NoSubtotals" sheetId="3" r:id="rId3"/>
     <sheet name="GrandTotals" sheetId="6" r:id="rId4"/>
+    <sheet name="MultipleDataFields" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId5"/>
+    <pivotCache cacheId="21" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="40">
   <si>
     <t>Transaction</t>
   </si>
@@ -118,6 +119,39 @@
   </si>
   <si>
     <t>Sum of Total</t>
+  </si>
+  <si>
+    <t>Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Total Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Total Sum of Total</t>
+  </si>
+  <si>
+    <t>Car Rack Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Car Rack Sum of Total</t>
+  </si>
+  <si>
+    <t>Headlamp Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Headlamp Sum of Total</t>
+  </si>
+  <si>
+    <t>Sleeping Bag Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Sleeping Bag Sum of Total</t>
+  </si>
+  <si>
+    <t>Tent Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Tent Sum of Total</t>
   </si>
 </sst>
 </file>
@@ -358,7 +392,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B12:R23" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -517,7 +551,85 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -570,8 +682,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L1:M17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -677,8 +789,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A26:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -753,86 +865,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:I13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -953,7 +987,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:L8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1049,6 +1083,219 @@
     </i>
   </colItems>
   <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{615E3895-2707-42E3-A785-8864A18E17EE}" name="MultipleDataFieldsPivotTable2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A10:W17" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="3">
+    <field x="3"/>
+    <field x="1"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="22">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i t="default" i="1">
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F81C657-F972-42B9-99B1-6B9FF9338C17}" name="MultipleDataFieldsPivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
     <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1362,7 +1609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86234C7-1633-473D-AAFD-744E7802C65D}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2514,7 +2761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2B0220-1F7B-4702-A332-D90617B220D1}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2726,4 +2973,421 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1988C9-490B-47F1-9FDF-A00AFE8AC1EA}">
+  <dimension ref="A1:W17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>37</v>
+      </c>
+      <c r="R11" t="s">
+        <v>16</v>
+      </c>
+      <c r="T11" t="s">
+        <v>38</v>
+      </c>
+      <c r="U11" t="s">
+        <v>39</v>
+      </c>
+      <c r="V11" t="s">
+        <v>30</v>
+      </c>
+      <c r="W11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" t="s">
+        <v>7</v>
+      </c>
+      <c r="R12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" t="s">
+        <v>29</v>
+      </c>
+      <c r="S13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H14" s="4">
+        <v>5</v>
+      </c>
+      <c r="I14" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4">
+        <v>5</v>
+      </c>
+      <c r="W14" s="4">
+        <v>2078.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4">
+        <v>1</v>
+      </c>
+      <c r="O15" s="4">
+        <v>99</v>
+      </c>
+      <c r="P15" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>99</v>
+      </c>
+      <c r="R15" s="4">
+        <v>6</v>
+      </c>
+      <c r="S15" s="4">
+        <v>1194</v>
+      </c>
+      <c r="T15" s="4">
+        <v>6</v>
+      </c>
+      <c r="U15" s="4">
+        <v>1194</v>
+      </c>
+      <c r="V15" s="4">
+        <v>7</v>
+      </c>
+      <c r="W15" s="4">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4">
+        <v>2</v>
+      </c>
+      <c r="I16" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1</v>
+      </c>
+      <c r="M16" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4">
+        <v>3</v>
+      </c>
+      <c r="W16" s="4">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="D17" s="4">
+        <v>4</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1663</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H17" s="4">
+        <v>7</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2910.25</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="L17" s="4">
+        <v>1</v>
+      </c>
+      <c r="M17" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="N17" s="4">
+        <v>1</v>
+      </c>
+      <c r="O17" s="4">
+        <v>99</v>
+      </c>
+      <c r="P17" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>99</v>
+      </c>
+      <c r="R17" s="4">
+        <v>6</v>
+      </c>
+      <c r="S17" s="4">
+        <v>1194</v>
+      </c>
+      <c r="T17" s="4">
+        <v>6</v>
+      </c>
+      <c r="U17" s="4">
+        <v>1194</v>
+      </c>
+      <c r="V17" s="4">
+        <v>15</v>
+      </c>
+      <c r="W17" s="4">
+        <v>4228.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Abstracted method for building row items.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
+++ b/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{29B48D6B-EB98-4495-86AA-5E6829495C1A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E264EB76-EFF3-49C7-B9D3-33E620B2CAF3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22416" windowHeight="10476" activeTab="4" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9756" activeTab="5" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="NoSubtotals" sheetId="3" r:id="rId3"/>
     <sheet name="GrandTotals" sheetId="6" r:id="rId4"/>
     <sheet name="MultipleDataFields" sheetId="7" r:id="rId5"/>
+    <sheet name="RowDataFields" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId6"/>
+    <pivotCache cacheId="12" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="46">
   <si>
     <t>Transaction</t>
   </si>
@@ -153,6 +154,24 @@
   <si>
     <t>Tent Sum of Total</t>
   </si>
+  <si>
+    <t>Chicago Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Chicago Sum of Total</t>
+  </si>
+  <si>
+    <t>Nashville Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>Nashville Sum of Total</t>
+  </si>
+  <si>
+    <t>San Francisco Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>San Francisco Sum of Total</t>
+  </si>
 </sst>
 </file>
 
@@ -227,7 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -243,6 +262,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -302,7 +324,12 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Wholesale Price" numFmtId="8">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="24.99" maxValue="415.75"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="24.99" maxValue="415.75" count="4">
+        <n v="415.75"/>
+        <n v="99"/>
+        <n v="24.99"/>
+        <n v="199"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Units Sold" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6" count="3">
@@ -330,7 +357,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="415.75"/>
+    <x v="0"/>
     <x v="0"/>
     <n v="415.75"/>
   </r>
@@ -339,7 +366,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <n v="99"/>
+    <x v="1"/>
     <x v="0"/>
     <n v="99"/>
   </r>
@@ -348,7 +375,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-    <n v="24.99"/>
+    <x v="2"/>
     <x v="0"/>
     <n v="24.99"/>
   </r>
@@ -357,7 +384,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="415.75"/>
+    <x v="0"/>
     <x v="1"/>
     <n v="831.5"/>
   </r>
@@ -366,7 +393,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="3"/>
-    <n v="199"/>
+    <x v="3"/>
     <x v="2"/>
     <n v="1194"/>
   </r>
@@ -375,7 +402,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="0"/>
-    <n v="415.75"/>
+    <x v="0"/>
     <x v="1"/>
     <n v="831.5"/>
   </r>
@@ -384,7 +411,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="415.75"/>
+    <x v="0"/>
     <x v="1"/>
     <n v="831.5"/>
   </r>
@@ -392,7 +419,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B12:R23" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -550,13 +577,31 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C74FC5-394B-4FAE-AEC0-2D1A8752CE1D}" name="RowDataFieldsPivotTable3" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="O1:S52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
@@ -564,7 +609,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
       <items count="5">
         <item x="0"/>
         <item x="2"/>
@@ -573,47 +618,285 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="1"/>
+    <field x="3"/>
+    <field x="0"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="50">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="3"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1CE963B4-85F1-470B-8720-5625E53AD926}" name="RowDataFieldsPivotTable1" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" numFmtId="8" showAll="0"/>
   </pivotFields>
   <rowFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
     <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
       <x v="2"/>
     </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
     <i t="grand">
       <x/>
     </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
-  <dataFields count="1">
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
     <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -628,13 +911,20 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BBD4942-F2DC-4306-B86C-66D12FC3A0F1}" name="RowDataFieldsPivotTable2" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="H1:L31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
@@ -642,15 +932,117 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="3">
+    <field x="1"/>
+    <field x="3"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="29">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
     <field x="2"/>
-  </rowFields>
-  <rowItems count="4">
+  </colFields>
+  <colItems count="4">
     <i>
       <x/>
     </i>
@@ -663,11 +1055,9 @@
     <i t="grand">
       <x/>
     </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
-  <dataFields count="1">
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
     <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -676,14 +1066,14 @@
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L1:M17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -789,8 +1179,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A26:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -865,8 +1255,140 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:I13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -987,7 +1509,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:L8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1098,7 +1620,70 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{615E3895-2707-42E3-A785-8864A18E17EE}" name="MultipleDataFieldsPivotTable2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F81C657-F972-42B9-99B1-6B9FF9338C17}" name="MultipleDataFieldsPivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{615E3895-2707-42E3-A785-8864A18E17EE}" name="MultipleDataFieldsPivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A10:W17" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1229,69 +1814,6 @@
     </i>
     <i t="grand" i="1">
       <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F81C657-F972-42B9-99B1-6B9FF9338C17}" name="MultipleDataFieldsPivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
     </i>
   </colItems>
   <dataFields count="2">
@@ -2979,7 +3501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1988C9-490B-47F1-9FDF-A00AFE8AC1EA}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -3390,4 +3912,1159 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ACBDB8F-63DE-4712-8264-42C0117CE607}">
+  <dimension ref="A1:S52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58:J60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="H3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="O3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="O4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="E5" s="4">
+        <v>856.49</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="4">
+        <v>2</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4">
+        <v>2</v>
+      </c>
+      <c r="O5" s="7">
+        <v>20100007</v>
+      </c>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="H6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>10</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="O7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1194</v>
+      </c>
+      <c r="D8" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2857</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="H9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="L9" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="4">
+        <v>2</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
+        <v>3</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="C11" s="4">
+        <v>99</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4">
+        <v>514.75</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="L11" s="4">
+        <v>856.49</v>
+      </c>
+      <c r="O11" s="7">
+        <v>20100083</v>
+      </c>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>15</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="O12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4">
+        <v>1</v>
+      </c>
+      <c r="S12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1293</v>
+      </c>
+      <c r="D13" s="4">
+        <v>856.49</v>
+      </c>
+      <c r="E13" s="4">
+        <v>4228.24</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="O13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="S13" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="H14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="4">
+        <v>2</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4">
+        <v>2</v>
+      </c>
+      <c r="L14" s="4">
+        <v>4</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4">
+        <v>1</v>
+      </c>
+      <c r="S14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="H15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1663</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="S15" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="H16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="O16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P16" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4">
+        <v>1</v>
+      </c>
+      <c r="S16" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4">
+        <v>6</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4">
+        <v>6</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P17" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="S17" s="4">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="18" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H18" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4">
+        <v>1194</v>
+      </c>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4">
+        <v>1194</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+    </row>
+    <row r="19" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2</v>
+      </c>
+      <c r="J19" s="4">
+        <v>6</v>
+      </c>
+      <c r="K19" s="4">
+        <v>2</v>
+      </c>
+      <c r="L19" s="4">
+        <v>10</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+    </row>
+    <row r="20" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1194</v>
+      </c>
+      <c r="K20" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="L20" s="4">
+        <v>2857</v>
+      </c>
+      <c r="O20" s="7">
+        <v>20100017</v>
+      </c>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+    </row>
+    <row r="21" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="O21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4">
+        <v>2</v>
+      </c>
+      <c r="S21" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="O22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="S22" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="23" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4">
+        <v>1</v>
+      </c>
+      <c r="O23" s="7">
+        <v>20100090</v>
+      </c>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+    </row>
+    <row r="24" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="O25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="26" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4">
+        <v>1</v>
+      </c>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4">
+        <v>1</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P26" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4">
+        <v>2</v>
+      </c>
+      <c r="S26" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4">
+        <v>99</v>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4">
+        <v>99</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P27" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="S27" s="4">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="28" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28" s="4">
+        <v>1</v>
+      </c>
+      <c r="J28" s="4">
+        <v>1</v>
+      </c>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4">
+        <v>2</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+    </row>
+    <row r="29" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="J29" s="4">
+        <v>99</v>
+      </c>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4">
+        <v>514.75</v>
+      </c>
+      <c r="O29" s="7">
+        <v>20100070</v>
+      </c>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+    </row>
+    <row r="30" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" s="4">
+        <v>5</v>
+      </c>
+      <c r="J30" s="4">
+        <v>7</v>
+      </c>
+      <c r="K30" s="4">
+        <v>3</v>
+      </c>
+      <c r="L30" s="4">
+        <v>15</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4">
+        <v>6</v>
+      </c>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="H31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="J31" s="4">
+        <v>1293</v>
+      </c>
+      <c r="K31" s="4">
+        <v>856.49</v>
+      </c>
+      <c r="L31" s="4">
+        <v>4228.24</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4">
+        <v>1194</v>
+      </c>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="32" spans="8:19" x14ac:dyDescent="0.3">
+      <c r="O32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4">
+        <v>6</v>
+      </c>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O33" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4">
+        <v>1194</v>
+      </c>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="34" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P34" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>6</v>
+      </c>
+      <c r="R34" s="4">
+        <v>2</v>
+      </c>
+      <c r="S34" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P35" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>1194</v>
+      </c>
+      <c r="R35" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="S35" s="4">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="36" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+    </row>
+    <row r="37" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+    </row>
+    <row r="38" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O38" s="7">
+        <v>20100076</v>
+      </c>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+    </row>
+    <row r="39" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O39" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P39" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O40" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P40" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="41" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O41" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P41" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O42" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P42" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="43" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O43" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+    </row>
+    <row r="44" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O44" s="7">
+        <v>20100085</v>
+      </c>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+    </row>
+    <row r="45" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O45" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4">
+        <v>1</v>
+      </c>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O46" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4">
+        <v>99</v>
+      </c>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O47" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4">
+        <v>1</v>
+      </c>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O48" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4">
+        <v>99</v>
+      </c>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O49" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P49" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="4">
+        <v>1</v>
+      </c>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O50" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P50" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>99</v>
+      </c>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="51" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O51" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P51" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>7</v>
+      </c>
+      <c r="R51" s="4">
+        <v>3</v>
+      </c>
+      <c r="S51" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O52" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P52" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="Q52" s="4">
+        <v>1293</v>
+      </c>
+      <c r="R52" s="4">
+        <v>856.49</v>
+      </c>
+      <c r="S52" s="4">
+        <v>4228.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added support for pivot tables with multiple row data fields and no column fields.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
+++ b/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E264EB76-EFF3-49C7-B9D3-33E620B2CAF3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{58124507-CBFC-4C73-8408-6496CA9DA9DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9756" activeTab="5" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId7"/>
+    <pivotCache cacheId="29" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="52">
   <si>
     <t>Transaction</t>
   </si>
@@ -171,6 +171,24 @@
   </si>
   <si>
     <t>San Francisco Sum of Total</t>
+  </si>
+  <si>
+    <t>January Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>January Sum of Total</t>
+  </si>
+  <si>
+    <t>February Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>February Sum of Total</t>
+  </si>
+  <si>
+    <t>March Sum of Units Sold</t>
+  </si>
+  <si>
+    <t>March Sum of Total</t>
   </si>
 </sst>
 </file>
@@ -419,7 +437,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B12:R23" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -578,7 +596,488 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C74FC5-394B-4FAE-AEC0-2D1A8752CE1D}" name="RowDataFieldsPivotTable3" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{275DFB84-4379-4C29-BE52-6943E478166B}" name="RowDataFieldsPivotTable5" cacheId="29" dataOnRows="1" dataPosition="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E37:F68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="31">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1CE963B4-85F1-470B-8720-5625E53AD926}" name="RowDataFieldsPivotTable1" cacheId="29" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1424B5F-181C-42B4-9454-6AAB7169E02E}" name="RowDataFieldsPivotTable4" cacheId="29" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A37:B48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BBD4942-F2DC-4306-B86C-66D12FC3A0F1}" name="RowDataFieldsPivotTable2" cacheId="29" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="H1:L31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="1"/>
+    <field x="3"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="29">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C74FC5-394B-4FAE-AEC0-2D1A8752CE1D}" name="RowDataFieldsPivotTable3" cacheId="29" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O1:S52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" subtotalTop="0" showAll="0">
@@ -813,20 +1312,13 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1CE963B4-85F1-470B-8720-5625E53AD926}" name="RowDataFieldsPivotTable1" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
@@ -836,67 +1328,30 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" numFmtId="8" showAll="0"/>
   </pivotFields>
-  <rowFields count="2">
-    <field x="1"/>
-    <field x="-2"/>
+  <rowFields count="1">
+    <field x="2"/>
   </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
       <x v="1"/>
     </i>
     <i>
       <x v="2"/>
     </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
     <i t="grand">
       <x/>
     </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
   </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+  <dataFields count="1">
     <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -911,169 +1366,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BBD4942-F2DC-4306-B86C-66D12FC3A0F1}" name="RowDataFieldsPivotTable2" cacheId="12" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="H1:L31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="1"/>
-    <field x="3"/>
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="29">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i t="default" i="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i t="default" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="default" i="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L1:M17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1179,8 +1473,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A26:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -1255,8 +1549,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1333,62 +1627,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:I13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -1509,7 +1749,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:L8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1620,70 +1860,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F81C657-F972-42B9-99B1-6B9FF9338C17}" name="MultipleDataFieldsPivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{615E3895-2707-42E3-A785-8864A18E17EE}" name="MultipleDataFieldsPivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{615E3895-2707-42E3-A785-8864A18E17EE}" name="MultipleDataFieldsPivotTable2" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A10:W17" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1814,6 +1991,69 @@
     </i>
     <i t="grand" i="1">
       <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F81C657-F972-42B9-99B1-6B9FF9338C17}" name="MultipleDataFieldsPivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
     </i>
   </colItems>
   <dataFields count="2">
@@ -3916,20 +4156,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ACBDB8F-63DE-4712-8264-42C0117CE607}">
-  <dimension ref="A1:S52"/>
+  <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58:J60"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -4804,7 +5045,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="O33" s="6" t="s">
         <v>39</v>
       </c>
@@ -4817,7 +5058,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="34" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="O34" s="3" t="s">
         <v>42</v>
       </c>
@@ -4834,7 +5075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="O35" s="3" t="s">
         <v>43</v>
       </c>
@@ -4851,7 +5092,7 @@
         <v>2857</v>
       </c>
     </row>
-    <row r="36" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="O36" s="3" t="s">
         <v>7</v>
       </c>
@@ -4860,7 +5101,13 @@
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
     </row>
-    <row r="37" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="O37" s="6" t="s">
         <v>9</v>
       </c>
@@ -4869,7 +5116,15 @@
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
     </row>
-    <row r="38" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="E38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="4"/>
       <c r="O38" s="7">
         <v>20100076</v>
       </c>
@@ -4878,7 +5133,17 @@
       <c r="R38" s="4"/>
       <c r="S38" s="4"/>
     </row>
-    <row r="39" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="4">
+        <v>5</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="4"/>
       <c r="O39" s="8" t="s">
         <v>29</v>
       </c>
@@ -4891,7 +5156,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="4">
+        <v>2078.75</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="4">
+        <v>2</v>
+      </c>
       <c r="O40" s="8" t="s">
         <v>28</v>
       </c>
@@ -4904,7 +5181,17 @@
         <v>415.75</v>
       </c>
     </row>
-    <row r="41" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="E41" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="4">
+        <v>2</v>
+      </c>
       <c r="O41" s="6" t="s">
         <v>32</v>
       </c>
@@ -4917,7 +5204,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="4">
+        <v>7</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="4">
+        <v>1</v>
+      </c>
       <c r="O42" s="6" t="s">
         <v>33</v>
       </c>
@@ -4930,7 +5229,17 @@
         <v>415.75</v>
       </c>
     </row>
-    <row r="43" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1293</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" s="4"/>
       <c r="O43" s="6" t="s">
         <v>11</v>
       </c>
@@ -4939,7 +5248,17 @@
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
     </row>
-    <row r="44" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="E44" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="4">
+        <v>831.5</v>
+      </c>
       <c r="O44" s="7">
         <v>20100085</v>
       </c>
@@ -4948,7 +5267,19 @@
       <c r="R44" s="4"/>
       <c r="S44" s="4"/>
     </row>
-    <row r="45" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" s="4">
+        <v>3</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="4">
+        <v>831.5</v>
+      </c>
       <c r="O45" s="8" t="s">
         <v>29</v>
       </c>
@@ -4961,7 +5292,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="4">
+        <v>856.49</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="4">
+        <v>415.75</v>
+      </c>
       <c r="O46" s="8" t="s">
         <v>28</v>
       </c>
@@ -4974,7 +5317,19 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="4">
+        <v>15</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47" s="4">
+        <v>5</v>
+      </c>
       <c r="O47" s="6" t="s">
         <v>36</v>
       </c>
@@ -4987,7 +5342,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="4">
+        <v>4228.24</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" s="4">
+        <v>2078.75</v>
+      </c>
       <c r="O48" s="6" t="s">
         <v>37</v>
       </c>
@@ -5000,7 +5367,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="4"/>
       <c r="O49" s="3" t="s">
         <v>44</v>
       </c>
@@ -5015,7 +5386,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E50" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" s="4"/>
       <c r="O50" s="3" t="s">
         <v>45</v>
       </c>
@@ -5030,7 +5405,13 @@
         <v>514.75</v>
       </c>
     </row>
-    <row r="51" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E51" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="4">
+        <v>6</v>
+      </c>
       <c r="O51" s="3" t="s">
         <v>30</v>
       </c>
@@ -5047,7 +5428,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E52" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="4">
+        <v>1</v>
+      </c>
       <c r="O52" s="3" t="s">
         <v>31</v>
       </c>
@@ -5061,6 +5448,126 @@
         <v>856.49</v>
       </c>
       <c r="S52" s="4">
+        <v>4228.24</v>
+      </c>
+    </row>
+    <row r="53" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E53" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E54" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="4">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="55" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E56" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F56" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E57" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F57" s="4">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="58" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E58" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E59" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E60" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E61" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E62" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E63" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="64" spans="5:19" x14ac:dyDescent="0.3">
+      <c r="E64" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" s="4">
+        <v>831.5</v>
+      </c>
+    </row>
+    <row r="65" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E65" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F65" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E66" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F66" s="4">
+        <v>856.49</v>
+      </c>
+    </row>
+    <row r="67" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E67" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F67" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E68" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F68" s="4">
         <v>4228.24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
First pass of cleaning up column items and supporting multiple data fields in columns.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
+++ b/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{58124507-CBFC-4C73-8408-6496CA9DA9DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{502E345E-A7D4-4C88-B8E7-AC2ECC5C13C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9756" activeTab="5" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9756" firstSheet="6" activeTab="6" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,11 @@
     <sheet name="GrandTotals" sheetId="6" r:id="rId4"/>
     <sheet name="MultipleDataFields" sheetId="7" r:id="rId5"/>
     <sheet name="RowDataFields" sheetId="8" r:id="rId6"/>
+    <sheet name="ColumnDataFields" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="29" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="59">
   <si>
     <t>Transaction</t>
   </si>
@@ -189,6 +190,27 @@
   </si>
   <si>
     <t>March Sum of Total</t>
+  </si>
+  <si>
+    <t>Total Sum of Wholesale Price</t>
+  </si>
+  <si>
+    <t>January Sum of Wholesale Price</t>
+  </si>
+  <si>
+    <t>February Sum of Wholesale Price</t>
+  </si>
+  <si>
+    <t>March Sum of Wholesale Price</t>
+  </si>
+  <si>
+    <t>Chicago Total</t>
+  </si>
+  <si>
+    <t>Nashville Total</t>
+  </si>
+  <si>
+    <t>San Francisco Total</t>
   </si>
 </sst>
 </file>
@@ -437,7 +459,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B12:R23" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -596,250 +618,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{275DFB84-4379-4C29-BE52-6943E478166B}" name="RowDataFieldsPivotTable5" cacheId="29" dataOnRows="1" dataPosition="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E37:F68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="2"/>
-    <field x="-2"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="31">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i t="default" i="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i t="default" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="default" i="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1CE963B4-85F1-470B-8720-5625E53AD926}" name="RowDataFieldsPivotTable1" cacheId="29" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="1"/>
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1424B5F-181C-42B4-9454-6AAB7169E02E}" name="RowDataFieldsPivotTable4" cacheId="29" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1424B5F-181C-42B4-9454-6AAB7169E02E}" name="RowDataFieldsPivotTable4" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A37:B48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -915,8 +694,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BBD4942-F2DC-4306-B86C-66D12FC3A0F1}" name="RowDataFieldsPivotTable2" cacheId="29" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BBD4942-F2DC-4306-B86C-66D12FC3A0F1}" name="RowDataFieldsPivotTable2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H1:L31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -1076,8 +855,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C74FC5-394B-4FAE-AEC0-2D1A8752CE1D}" name="RowDataFieldsPivotTable3" cacheId="29" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C74FC5-394B-4FAE-AEC0-2D1A8752CE1D}" name="RowDataFieldsPivotTable3" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O1:S52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" subtotalTop="0" showAll="0">
@@ -1312,8 +1091,965 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{275DFB84-4379-4C29-BE52-6943E478166B}" name="RowDataFieldsPivotTable5" cacheId="1" dataOnRows="1" dataPosition="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E37:F68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="31">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1CE963B4-85F1-470B-8720-5625E53AD926}" name="RowDataFieldsPivotTable1" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{66A9754B-81DC-4ED4-A80A-016D7E514761}" name="ColumnDataFieldsPivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:I7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{89F6948F-8455-4692-97DB-D9DBCCE61BCB}" name="ColumnDataFieldsPivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A21:S28" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="3">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="18">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3118B986-EAC5-4497-83A8-B5E3225EEBB6}" name="ColumnDataFieldsPivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A11:I17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="-2"/>
+    <field x="2"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB40D58C-DD49-4477-9AD2-60BBD9C1D8DD}" name="ColumnDataFieldsPivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A59:Q71" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="7">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="4">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="1"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="16">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43B65DE5-75DB-4432-AD36-D0F632525498}" name="ColumnDataFieldsPivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A43:AK55" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="4">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="1"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="36">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i t="default" r="2">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default" r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i t="default" r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i t="default" r="2">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i t="default" r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i t="default" r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i t="default" r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default" r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1366,8 +2102,124 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D539B62D-4AC8-46E3-A8D4-1D8AFFC11145}" name="ColumnDataFieldsPivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A32:M39" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="3">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="12">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L1:M17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1474,7 +2326,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A26:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -1550,7 +2402,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1628,7 +2480,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:I13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -1749,7 +2601,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:L8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1860,7 +2712,70 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{615E3895-2707-42E3-A785-8864A18E17EE}" name="MultipleDataFieldsPivotTable2" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F81C657-F972-42B9-99B1-6B9FF9338C17}" name="MultipleDataFieldsPivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{615E3895-2707-42E3-A785-8864A18E17EE}" name="MultipleDataFieldsPivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A10:W17" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1991,69 +2906,6 @@
     </i>
     <i t="grand" i="1">
       <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F81C657-F972-42B9-99B1-6B9FF9338C17}" name="MultipleDataFieldsPivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
     </i>
   </colItems>
   <dataFields count="2">
@@ -3741,9 +4593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1988C9-490B-47F1-9FDF-A00AFE8AC1EA}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4158,7 +5008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ACBDB8F-63DE-4712-8264-42C0117CE607}">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
@@ -5574,4 +6424,1972 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE2431C-D3CF-40A9-83CD-D04719B9BC4E}">
+  <dimension ref="A1:AK71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="27" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="27" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="H4" s="4">
+        <v>3</v>
+      </c>
+      <c r="I4" s="4">
+        <v>440.74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D5" s="4">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4">
+        <v>199</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H5" s="4">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1030.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>99</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
+        <v>2</v>
+      </c>
+      <c r="I6" s="4">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1247.25</v>
+      </c>
+      <c r="D7" s="4">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4">
+        <v>298</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4">
+        <v>440.74</v>
+      </c>
+      <c r="H7" s="4">
+        <v>15</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1985.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="H14" s="4">
+        <v>3</v>
+      </c>
+      <c r="I14" s="4">
+        <v>440.74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4">
+        <v>6</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F15" s="4">
+        <v>199</v>
+      </c>
+      <c r="G15" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H15" s="4">
+        <v>10</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1030.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F16" s="4">
+        <v>99</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4">
+        <v>2</v>
+      </c>
+      <c r="I16" s="4">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="4">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4">
+        <v>7</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1247.25</v>
+      </c>
+      <c r="F17" s="4">
+        <v>298</v>
+      </c>
+      <c r="G17" s="4">
+        <v>440.74</v>
+      </c>
+      <c r="H17" s="4">
+        <v>15</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1985.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" t="s">
+        <v>54</v>
+      </c>
+      <c r="L22" t="s">
+        <v>13</v>
+      </c>
+      <c r="P22" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>55</v>
+      </c>
+      <c r="R22" t="s">
+        <v>30</v>
+      </c>
+      <c r="S22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" t="s">
+        <v>29</v>
+      </c>
+      <c r="N23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" t="s">
+        <v>9</v>
+      </c>
+      <c r="M24" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="4">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4">
+        <v>1</v>
+      </c>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="P25" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="R25" s="4">
+        <v>3</v>
+      </c>
+      <c r="S25" s="4">
+        <v>440.74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="4">
+        <v>2</v>
+      </c>
+      <c r="C26" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2</v>
+      </c>
+      <c r="E26" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4">
+        <v>6</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4">
+        <v>199</v>
+      </c>
+      <c r="J26" s="4">
+        <v>6</v>
+      </c>
+      <c r="K26" s="4">
+        <v>199</v>
+      </c>
+      <c r="L26" s="4">
+        <v>2</v>
+      </c>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="R26" s="4">
+        <v>10</v>
+      </c>
+      <c r="S26" s="4">
+        <v>1030.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4">
+        <v>99</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4">
+        <v>1</v>
+      </c>
+      <c r="K27" s="4">
+        <v>99</v>
+      </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4">
+        <v>2</v>
+      </c>
+      <c r="S27" s="4">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="4">
+        <v>5</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1247.25</v>
+      </c>
+      <c r="D28" s="4">
+        <v>5</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1247.25</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4">
+        <v>6</v>
+      </c>
+      <c r="H28" s="4">
+        <v>99</v>
+      </c>
+      <c r="I28" s="4">
+        <v>199</v>
+      </c>
+      <c r="J28" s="4">
+        <v>7</v>
+      </c>
+      <c r="K28" s="4">
+        <v>298</v>
+      </c>
+      <c r="L28" s="4">
+        <v>2</v>
+      </c>
+      <c r="M28" s="4">
+        <v>1</v>
+      </c>
+      <c r="N28" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="O28" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="P28" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>440.74</v>
+      </c>
+      <c r="R28" s="4">
+        <v>15</v>
+      </c>
+      <c r="S28" s="4">
+        <v>1985.99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" t="s">
+        <v>13</v>
+      </c>
+      <c r="L33" t="s">
+        <v>30</v>
+      </c>
+      <c r="M33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" t="s">
+        <v>29</v>
+      </c>
+      <c r="J34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" t="s">
+        <v>9</v>
+      </c>
+      <c r="K35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="4">
+        <v>2</v>
+      </c>
+      <c r="C36" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4">
+        <v>1</v>
+      </c>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="L36" s="4">
+        <v>3</v>
+      </c>
+      <c r="M36" s="4">
+        <v>440.74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="4">
+        <v>2</v>
+      </c>
+      <c r="C37" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4">
+        <v>6</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4">
+        <v>199</v>
+      </c>
+      <c r="H37" s="4">
+        <v>2</v>
+      </c>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4">
+        <v>10</v>
+      </c>
+      <c r="M37" s="4">
+        <v>1030.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4">
+        <v>99</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4">
+        <v>2</v>
+      </c>
+      <c r="M38" s="4">
+        <v>514.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="4">
+        <v>5</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1247.25</v>
+      </c>
+      <c r="D39" s="4">
+        <v>1</v>
+      </c>
+      <c r="E39" s="4">
+        <v>6</v>
+      </c>
+      <c r="F39" s="4">
+        <v>99</v>
+      </c>
+      <c r="G39" s="4">
+        <v>199</v>
+      </c>
+      <c r="H39" s="4">
+        <v>2</v>
+      </c>
+      <c r="I39" s="4">
+        <v>1</v>
+      </c>
+      <c r="J39" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="K39" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="L39" s="4">
+        <v>15</v>
+      </c>
+      <c r="M39" s="4">
+        <v>1985.99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="N44" t="s">
+        <v>46</v>
+      </c>
+      <c r="O44" t="s">
+        <v>53</v>
+      </c>
+      <c r="P44" t="s">
+        <v>10</v>
+      </c>
+      <c r="X44" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH44" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI44" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ44" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="H45" t="s">
+        <v>19</v>
+      </c>
+      <c r="P45" t="s">
+        <v>29</v>
+      </c>
+      <c r="T45" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" t="s">
+        <v>57</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" t="s">
+        <v>58</v>
+      </c>
+      <c r="H46" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" t="s">
+        <v>56</v>
+      </c>
+      <c r="J46" t="s">
+        <v>15</v>
+      </c>
+      <c r="K46" t="s">
+        <v>57</v>
+      </c>
+      <c r="L46" t="s">
+        <v>7</v>
+      </c>
+      <c r="M46" t="s">
+        <v>58</v>
+      </c>
+      <c r="P46" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>57</v>
+      </c>
+      <c r="R46" t="s">
+        <v>7</v>
+      </c>
+      <c r="S46" t="s">
+        <v>58</v>
+      </c>
+      <c r="T46" t="s">
+        <v>15</v>
+      </c>
+      <c r="U46" t="s">
+        <v>57</v>
+      </c>
+      <c r="V46" t="s">
+        <v>7</v>
+      </c>
+      <c r="W46" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" t="s">
+        <v>9</v>
+      </c>
+      <c r="J47" t="s">
+        <v>9</v>
+      </c>
+      <c r="L47" t="s">
+        <v>9</v>
+      </c>
+      <c r="P47" t="s">
+        <v>16</v>
+      </c>
+      <c r="R47" t="s">
+        <v>11</v>
+      </c>
+      <c r="T47" t="s">
+        <v>16</v>
+      </c>
+      <c r="V47" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>20100007</v>
+      </c>
+      <c r="B48" s="4">
+        <v>2</v>
+      </c>
+      <c r="C48" s="4">
+        <v>2</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="I48" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4">
+        <v>2</v>
+      </c>
+      <c r="O48" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="4"/>
+      <c r="X48" s="4"/>
+      <c r="Y48" s="4"/>
+      <c r="Z48" s="4"/>
+      <c r="AA48" s="4"/>
+      <c r="AB48" s="4"/>
+      <c r="AC48" s="4"/>
+      <c r="AD48" s="4"/>
+      <c r="AE48" s="4"/>
+      <c r="AF48" s="4"/>
+      <c r="AG48" s="4"/>
+      <c r="AH48" s="4"/>
+      <c r="AI48" s="4"/>
+      <c r="AJ48" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK48" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <v>20100017</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+      <c r="AB49" s="4">
+        <v>2</v>
+      </c>
+      <c r="AC49" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD49" s="4"/>
+      <c r="AE49" s="4"/>
+      <c r="AF49" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="AG49" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="AH49" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI49" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="AJ49" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK49" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <v>20100070</v>
+      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>6</v>
+      </c>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4">
+        <v>199</v>
+      </c>
+      <c r="U50" s="4">
+        <v>199</v>
+      </c>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="4">
+        <v>6</v>
+      </c>
+      <c r="Y50" s="4">
+        <v>199</v>
+      </c>
+      <c r="Z50" s="4"/>
+      <c r="AA50" s="4"/>
+      <c r="AB50" s="4"/>
+      <c r="AC50" s="4"/>
+      <c r="AD50" s="4"/>
+      <c r="AE50" s="4"/>
+      <c r="AF50" s="4"/>
+      <c r="AG50" s="4"/>
+      <c r="AH50" s="4"/>
+      <c r="AI50" s="4"/>
+      <c r="AJ50" s="4">
+        <v>6</v>
+      </c>
+      <c r="AK50" s="4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>20100076</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4">
+        <v>1</v>
+      </c>
+      <c r="G51" s="4">
+        <v>1</v>
+      </c>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="M51" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="N51" s="4">
+        <v>1</v>
+      </c>
+      <c r="O51" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4"/>
+      <c r="W51" s="4"/>
+      <c r="X51" s="4"/>
+      <c r="Y51" s="4"/>
+      <c r="Z51" s="4"/>
+      <c r="AA51" s="4"/>
+      <c r="AB51" s="4"/>
+      <c r="AC51" s="4"/>
+      <c r="AD51" s="4"/>
+      <c r="AE51" s="4"/>
+      <c r="AF51" s="4"/>
+      <c r="AG51" s="4"/>
+      <c r="AH51" s="4"/>
+      <c r="AI51" s="4"/>
+      <c r="AJ51" s="4">
+        <v>1</v>
+      </c>
+      <c r="AK51" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A52" s="3">
+        <v>20100083</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4"/>
+      <c r="X52" s="4"/>
+      <c r="Y52" s="4"/>
+      <c r="Z52" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA52" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB52" s="4"/>
+      <c r="AC52" s="4"/>
+      <c r="AD52" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="AE52" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="AF52" s="4"/>
+      <c r="AG52" s="4"/>
+      <c r="AH52" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI52" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="AJ52" s="4">
+        <v>1</v>
+      </c>
+      <c r="AK52" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
+        <v>20100085</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4">
+        <v>1</v>
+      </c>
+      <c r="S53" s="4">
+        <v>1</v>
+      </c>
+      <c r="T53" s="4"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="4">
+        <v>99</v>
+      </c>
+      <c r="W53" s="4">
+        <v>99</v>
+      </c>
+      <c r="X53" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y53" s="4">
+        <v>99</v>
+      </c>
+      <c r="Z53" s="4"/>
+      <c r="AA53" s="4"/>
+      <c r="AB53" s="4"/>
+      <c r="AC53" s="4"/>
+      <c r="AD53" s="4"/>
+      <c r="AE53" s="4"/>
+      <c r="AF53" s="4"/>
+      <c r="AG53" s="4"/>
+      <c r="AH53" s="4"/>
+      <c r="AI53" s="4"/>
+      <c r="AJ53" s="4">
+        <v>1</v>
+      </c>
+      <c r="AK53" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
+        <v>20100090</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4">
+        <v>2</v>
+      </c>
+      <c r="E54" s="4">
+        <v>2</v>
+      </c>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="K54" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4">
+        <v>2</v>
+      </c>
+      <c r="O54" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="4"/>
+      <c r="X54" s="4"/>
+      <c r="Y54" s="4"/>
+      <c r="Z54" s="4"/>
+      <c r="AA54" s="4"/>
+      <c r="AB54" s="4"/>
+      <c r="AC54" s="4"/>
+      <c r="AD54" s="4"/>
+      <c r="AE54" s="4"/>
+      <c r="AF54" s="4"/>
+      <c r="AG54" s="4"/>
+      <c r="AH54" s="4"/>
+      <c r="AI54" s="4"/>
+      <c r="AJ54" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK54" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="4">
+        <v>2</v>
+      </c>
+      <c r="C55" s="4">
+        <v>2</v>
+      </c>
+      <c r="D55" s="4">
+        <v>2</v>
+      </c>
+      <c r="E55" s="4">
+        <v>2</v>
+      </c>
+      <c r="F55" s="4">
+        <v>1</v>
+      </c>
+      <c r="G55" s="4">
+        <v>1</v>
+      </c>
+      <c r="H55" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="I55" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="J55" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="K55" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="L55" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="M55" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="N55" s="4">
+        <v>5</v>
+      </c>
+      <c r="O55" s="4">
+        <v>1247.25</v>
+      </c>
+      <c r="P55" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>6</v>
+      </c>
+      <c r="R55" s="4">
+        <v>1</v>
+      </c>
+      <c r="S55" s="4">
+        <v>1</v>
+      </c>
+      <c r="T55" s="4">
+        <v>199</v>
+      </c>
+      <c r="U55" s="4">
+        <v>199</v>
+      </c>
+      <c r="V55" s="4">
+        <v>99</v>
+      </c>
+      <c r="W55" s="4">
+        <v>99</v>
+      </c>
+      <c r="X55" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y55" s="4">
+        <v>298</v>
+      </c>
+      <c r="Z55" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA55" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB55" s="4">
+        <v>2</v>
+      </c>
+      <c r="AC55" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD55" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="AE55" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="AF55" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="AG55" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="AH55" s="4">
+        <v>3</v>
+      </c>
+      <c r="AI55" s="4">
+        <v>440.74</v>
+      </c>
+      <c r="AJ55" s="4">
+        <v>15</v>
+      </c>
+      <c r="AK55" s="4">
+        <v>1985.99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B59" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" t="s">
+        <v>10</v>
+      </c>
+      <c r="L60" t="s">
+        <v>13</v>
+      </c>
+      <c r="P60" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>29</v>
+      </c>
+      <c r="E61" t="s">
+        <v>19</v>
+      </c>
+      <c r="H61" t="s">
+        <v>29</v>
+      </c>
+      <c r="J61" t="s">
+        <v>19</v>
+      </c>
+      <c r="L61" t="s">
+        <v>29</v>
+      </c>
+      <c r="N61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" t="s">
+        <v>7</v>
+      </c>
+      <c r="J62" t="s">
+        <v>15</v>
+      </c>
+      <c r="K62" t="s">
+        <v>7</v>
+      </c>
+      <c r="L62" t="s">
+        <v>12</v>
+      </c>
+      <c r="M62" t="s">
+        <v>15</v>
+      </c>
+      <c r="N62" t="s">
+        <v>12</v>
+      </c>
+      <c r="O62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" t="s">
+        <v>9</v>
+      </c>
+      <c r="H63" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" t="s">
+        <v>11</v>
+      </c>
+      <c r="J63" t="s">
+        <v>16</v>
+      </c>
+      <c r="K63" t="s">
+        <v>11</v>
+      </c>
+      <c r="L63" t="s">
+        <v>14</v>
+      </c>
+      <c r="M63" t="s">
+        <v>9</v>
+      </c>
+      <c r="N63" t="s">
+        <v>14</v>
+      </c>
+      <c r="O63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
+        <v>20100007</v>
+      </c>
+      <c r="B64" s="4">
+        <v>2</v>
+      </c>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q64" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A65" s="3">
+        <v>20100017</v>
+      </c>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4">
+        <v>2</v>
+      </c>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P65" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q65" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
+        <v>20100070</v>
+      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4">
+        <v>6</v>
+      </c>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4">
+        <v>199</v>
+      </c>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q66" s="4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A67" s="3">
+        <v>20100076</v>
+      </c>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4">
+        <v>1</v>
+      </c>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A68" s="3">
+        <v>20100083</v>
+      </c>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4">
+        <v>1</v>
+      </c>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="O68" s="4"/>
+      <c r="P68" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A69" s="3">
+        <v>20100085</v>
+      </c>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4">
+        <v>1</v>
+      </c>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4">
+        <v>99</v>
+      </c>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A70" s="3">
+        <v>20100090</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4">
+        <v>2</v>
+      </c>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q70" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" s="4">
+        <v>2</v>
+      </c>
+      <c r="C71" s="4">
+        <v>2</v>
+      </c>
+      <c r="D71" s="4">
+        <v>1</v>
+      </c>
+      <c r="E71" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F71" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="G71" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H71" s="4">
+        <v>6</v>
+      </c>
+      <c r="I71" s="4">
+        <v>1</v>
+      </c>
+      <c r="J71" s="4">
+        <v>199</v>
+      </c>
+      <c r="K71" s="4">
+        <v>99</v>
+      </c>
+      <c r="L71" s="4">
+        <v>1</v>
+      </c>
+      <c r="M71" s="4">
+        <v>2</v>
+      </c>
+      <c r="N71" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="O71" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P71" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q71" s="4">
+        <v>1985.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more tests for column items with multiple data fields.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
+++ b/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{502E345E-A7D4-4C88-B8E7-AC2ECC5C13C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A5E68600-E034-46E6-98A3-7F4FACB72D61}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9756" firstSheet="6" activeTab="6" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9756" activeTab="6" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="10" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="62">
   <si>
     <t>Transaction</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>San Francisco Total</t>
+  </si>
+  <si>
+    <t>Chicago Sum of Wholesale Price</t>
+  </si>
+  <si>
+    <t>Nashville Sum of Wholesale Price</t>
+  </si>
+  <si>
+    <t>San Francisco Sum of Wholesale Price</t>
   </si>
 </sst>
 </file>
@@ -459,7 +468,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B12:R23" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -618,7 +627,250 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1424B5F-181C-42B4-9454-6AAB7169E02E}" name="RowDataFieldsPivotTable4" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{275DFB84-4379-4C29-BE52-6943E478166B}" name="RowDataFieldsPivotTable5" cacheId="10" dataOnRows="1" dataPosition="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E37:F68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="31">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1CE963B4-85F1-470B-8720-5625E53AD926}" name="RowDataFieldsPivotTable1" cacheId="10" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1424B5F-181C-42B4-9454-6AAB7169E02E}" name="RowDataFieldsPivotTable4" cacheId="10" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A37:B48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -694,8 +946,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BBD4942-F2DC-4306-B86C-66D12FC3A0F1}" name="RowDataFieldsPivotTable2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BBD4942-F2DC-4306-B86C-66D12FC3A0F1}" name="RowDataFieldsPivotTable2" cacheId="10" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H1:L31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -855,8 +1107,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C74FC5-394B-4FAE-AEC0-2D1A8752CE1D}" name="RowDataFieldsPivotTable3" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C74FC5-394B-4FAE-AEC0-2D1A8752CE1D}" name="RowDataFieldsPivotTable3" cacheId="10" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O1:S52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" subtotalTop="0" showAll="0">
@@ -1091,124 +1343,112 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{275DFB84-4379-4C29-BE52-6943E478166B}" name="RowDataFieldsPivotTable5" cacheId="1" dataOnRows="1" dataPosition="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E37:F68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80E6C19D-DBE6-4B69-B9AA-DAA44B187BF6}" name="ColumnDataFieldsPivotTable10" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A119:Q127" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
         <item x="1"/>
         <item x="2"/>
         <item x="0"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowFields count="3">
-    <field x="2"/>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="3">
     <field x="-2"/>
     <field x="1"/>
-  </rowFields>
-  <rowItems count="31">
-    <i>
-      <x/>
+    <field x="2"/>
+  </colFields>
+  <colItems count="16">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
     </i>
     <i r="1">
+      <x v="1"/>
       <x/>
     </i>
     <i r="2">
-      <x/>
+      <x v="1"/>
     </i>
     <i r="2">
-      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
     </i>
     <i r="2">
+      <x v="1"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
       <x v="2"/>
     </i>
     <i r="1" i="1">
       <x v="1"/>
+      <x/>
     </i>
     <i r="2" i="1">
-      <x/>
+      <x v="1"/>
     </i>
     <i r="2" i="1">
-      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+      <x/>
     </i>
     <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i t="default" i="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i t="default" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="default" i="1">
-      <x v="2"/>
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -1216,13 +1456,10 @@
     <i t="grand" i="1">
       <x/>
     </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
   <dataFields count="2">
     <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1230,18 +1467,18 @@
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1CE963B4-85F1-470B-8720-5625E53AD926}" name="RowDataFieldsPivotTable1" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E5F8A30F-D02F-44BC-8036-0AB6A3D95E00}" name="ColumnDataFieldsPivotTable9" cacheId="10" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A107:W115" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisCol" showAll="0">
       <items count="4">
         <item x="1"/>
         <item x="2"/>
@@ -1257,197 +1494,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="1"/>
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{66A9754B-81DC-4ED4-A80A-016D7E514761}" name="ColumnDataFieldsPivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:I7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="2"/>
-    <field x="-2"/>
-  </colFields>
-  <colItems count="8">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{89F6948F-8455-4692-97DB-D9DBCCE61BCB}" name="ColumnDataFieldsPivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A21:S28" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
       <items count="5">
         <item x="0"/>
         <item x="2"/>
@@ -1461,83 +1508,97 @@
     <pivotField numFmtId="8" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="1"/>
+    <field x="3"/>
   </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
   <colFields count="3">
+    <field x="-2"/>
+    <field x="1"/>
     <field x="2"/>
-    <field x="-2"/>
-    <field x="3"/>
   </colFields>
-  <colItems count="18">
-    <i>
-      <x/>
-      <x/>
+  <colItems count="22">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1" i="1">
       <x/>
     </i>
     <i r="1" i="1">
       <x v="1"/>
       <x/>
     </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i t="default" i="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="1"/>
     </i>
     <i r="1" i="1">
-      <x v="1"/>
-      <x v="2"/>
+      <x v="2"/>
+      <x/>
     </i>
     <i r="2" i="1">
-      <x v="3"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i t="default" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1" i="1">
       <x v="2"/>
     </i>
     <i t="grand">
@@ -1564,99 +1625,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3118B986-EAC5-4497-83A8-B5E3225EEBB6}" name="ColumnDataFieldsPivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A11:I17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="-2"/>
-    <field x="2"/>
-  </colFields>
-  <colItems count="8">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB40D58C-DD49-4477-9AD2-60BBD9C1D8DD}" name="ColumnDataFieldsPivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A59:Q71" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8A4BBC34-425D-4477-AA03-0141BD5FAAD9}" name="ColumnDataFieldsPivotTable8" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A91:Q103" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
       <items count="7">
@@ -1726,8 +1696,8 @@
   </rowItems>
   <colFields count="4">
     <field x="2"/>
+    <field x="1"/>
     <field x="-2"/>
-    <field x="1"/>
     <field x="3"/>
   </colFields>
   <colItems count="16">
@@ -1737,60 +1707,61 @@
       <x/>
       <x/>
     </i>
-    <i r="2">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x/>
-      <x/>
-    </i>
     <i r="2" i="1">
       <x v="1"/>
       <x/>
     </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
     <i r="2" i="1">
-      <x v="2"/>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="1"/>
+      <x/>
       <x v="3"/>
     </i>
-    <i r="2">
-      <x v="2"/>
-      <x v="2"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
+    <i r="2" i="1">
       <x v="1"/>
       <x v="3"/>
     </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+      <x v="2"/>
+    </i>
     <i r="2" i="1">
-      <x v="2"/>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+      <x/>
     </i>
     <i r="2" i="1">
       <x v="1"/>
@@ -1819,8 +1790,238 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{130E016C-4138-40D8-9FA8-D4183603FDA1}" name="ColumnDataFieldsPivotTable7" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A75:AK87" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="4">
+    <field x="2"/>
+    <field x="1"/>
+    <field x="-2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="36">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="1"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43B65DE5-75DB-4432-AD36-D0F632525498}" name="ColumnDataFieldsPivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43B65DE5-75DB-4432-AD36-D0F632525498}" name="ColumnDataFieldsPivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A43:AK55" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -2049,36 +2250,58 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A26:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
     <field x="2"/>
+    <field x="3"/>
   </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -2096,14 +2319,14 @@
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D539B62D-4AC8-46E3-A8D4-1D8AFFC11145}" name="ColumnDataFieldsPivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D539B62D-4AC8-46E3-A8D4-1D8AFFC11145}" name="ColumnDataFieldsPivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A32:M39" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -2218,8 +2441,625 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{66A9754B-81DC-4ED4-A80A-016D7E514761}" name="ColumnDataFieldsPivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:I7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{89F6948F-8455-4692-97DB-D9DBCCE61BCB}" name="ColumnDataFieldsPivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A21:S28" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="3">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="18">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3118B986-EAC5-4497-83A8-B5E3225EEBB6}" name="ColumnDataFieldsPivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A11:I17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="-2"/>
+    <field x="2"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB40D58C-DD49-4477-9AD2-60BBD9C1D8DD}" name="ColumnDataFieldsPivotTable6" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A59:Q71" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="7">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="4">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="1"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="16">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L1:M17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2325,162 +3165,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A26:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:I13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -2601,7 +3287,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:L8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2712,70 +3398,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F81C657-F972-42B9-99B1-6B9FF9338C17}" name="MultipleDataFieldsPivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{615E3895-2707-42E3-A785-8864A18E17EE}" name="MultipleDataFieldsPivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{615E3895-2707-42E3-A785-8864A18E17EE}" name="MultipleDataFieldsPivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A10:W17" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -2906,6 +3529,69 @@
     </i>
     <i t="grand" i="1">
       <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F81C657-F972-42B9-99B1-6B9FF9338C17}" name="MultipleDataFieldsPivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
     </i>
   </colItems>
   <dataFields count="2">
@@ -6428,68 +7114,65 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE2431C-D3CF-40A9-83CD-D04719B9BC4E}">
-  <dimension ref="A1:AK71"/>
+  <dimension ref="A1:AK127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="29" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="27" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="43" max="45" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="29.109375" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="27" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="27" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="25.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -8162,7 +8845,7 @@
         <v>415.75</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>20100017</v>
       </c>
@@ -8191,7 +8874,7 @@
         <v>415.75</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>20100070</v>
       </c>
@@ -8220,7 +8903,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>20100076</v>
       </c>
@@ -8249,7 +8932,7 @@
         <v>415.75</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>20100083</v>
       </c>
@@ -8278,7 +8961,7 @@
         <v>24.99</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>20100085</v>
       </c>
@@ -8307,7 +8990,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>20100090</v>
       </c>
@@ -8336,7 +9019,7 @@
         <v>415.75</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>18</v>
       </c>
@@ -8386,6 +9069,1724 @@
         <v>15</v>
       </c>
       <c r="Q71" s="4">
+        <v>1985.99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B75" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="N76" t="s">
+        <v>46</v>
+      </c>
+      <c r="O76" t="s">
+        <v>53</v>
+      </c>
+      <c r="P76" t="s">
+        <v>10</v>
+      </c>
+      <c r="X76" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z76" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH76" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI76" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ76" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK76" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" t="s">
+        <v>40</v>
+      </c>
+      <c r="E77" t="s">
+        <v>59</v>
+      </c>
+      <c r="F77" t="s">
+        <v>15</v>
+      </c>
+      <c r="H77" t="s">
+        <v>42</v>
+      </c>
+      <c r="I77" t="s">
+        <v>60</v>
+      </c>
+      <c r="J77" t="s">
+        <v>7</v>
+      </c>
+      <c r="L77" t="s">
+        <v>44</v>
+      </c>
+      <c r="M77" t="s">
+        <v>61</v>
+      </c>
+      <c r="P77" t="s">
+        <v>15</v>
+      </c>
+      <c r="R77" t="s">
+        <v>42</v>
+      </c>
+      <c r="S77" t="s">
+        <v>60</v>
+      </c>
+      <c r="T77" t="s">
+        <v>7</v>
+      </c>
+      <c r="V77" t="s">
+        <v>44</v>
+      </c>
+      <c r="W77" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC77" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD77" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF77" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG77" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78" t="s">
+        <v>19</v>
+      </c>
+      <c r="F78" t="s">
+        <v>29</v>
+      </c>
+      <c r="G78" t="s">
+        <v>19</v>
+      </c>
+      <c r="J78" t="s">
+        <v>29</v>
+      </c>
+      <c r="K78" t="s">
+        <v>19</v>
+      </c>
+      <c r="P78" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>19</v>
+      </c>
+      <c r="T78" t="s">
+        <v>29</v>
+      </c>
+      <c r="U78" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z78" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA78" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD78" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE78" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" t="s">
+        <v>9</v>
+      </c>
+      <c r="G79" t="s">
+        <v>9</v>
+      </c>
+      <c r="J79" t="s">
+        <v>9</v>
+      </c>
+      <c r="K79" t="s">
+        <v>9</v>
+      </c>
+      <c r="P79" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>16</v>
+      </c>
+      <c r="T79" t="s">
+        <v>11</v>
+      </c>
+      <c r="U79" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z79" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA79" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD79" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A80" s="3">
+        <v>20100007</v>
+      </c>
+      <c r="B80" s="4">
+        <v>2</v>
+      </c>
+      <c r="C80" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D80" s="4">
+        <v>2</v>
+      </c>
+      <c r="E80" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4">
+        <v>2</v>
+      </c>
+      <c r="O80" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
+      <c r="S80" s="4"/>
+      <c r="T80" s="4"/>
+      <c r="U80" s="4"/>
+      <c r="V80" s="4"/>
+      <c r="W80" s="4"/>
+      <c r="X80" s="4"/>
+      <c r="Y80" s="4"/>
+      <c r="Z80" s="4"/>
+      <c r="AA80" s="4"/>
+      <c r="AB80" s="4"/>
+      <c r="AC80" s="4"/>
+      <c r="AD80" s="4"/>
+      <c r="AE80" s="4"/>
+      <c r="AF80" s="4"/>
+      <c r="AG80" s="4"/>
+      <c r="AH80" s="4"/>
+      <c r="AI80" s="4"/>
+      <c r="AJ80" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK80" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
+        <v>20100017</v>
+      </c>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="4"/>
+      <c r="S81" s="4"/>
+      <c r="T81" s="4"/>
+      <c r="U81" s="4"/>
+      <c r="V81" s="4"/>
+      <c r="W81" s="4"/>
+      <c r="X81" s="4"/>
+      <c r="Y81" s="4"/>
+      <c r="Z81" s="4"/>
+      <c r="AA81" s="4"/>
+      <c r="AB81" s="4"/>
+      <c r="AC81" s="4"/>
+      <c r="AD81" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE81" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="AF81" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG81" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="AH81" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI81" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="AJ81" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK81" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A82" s="3">
+        <v>20100070</v>
+      </c>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q82" s="4">
+        <v>199</v>
+      </c>
+      <c r="R82" s="4">
+        <v>6</v>
+      </c>
+      <c r="S82" s="4">
+        <v>199</v>
+      </c>
+      <c r="T82" s="4"/>
+      <c r="U82" s="4"/>
+      <c r="V82" s="4"/>
+      <c r="W82" s="4"/>
+      <c r="X82" s="4">
+        <v>6</v>
+      </c>
+      <c r="Y82" s="4">
+        <v>199</v>
+      </c>
+      <c r="Z82" s="4"/>
+      <c r="AA82" s="4"/>
+      <c r="AB82" s="4"/>
+      <c r="AC82" s="4"/>
+      <c r="AD82" s="4"/>
+      <c r="AE82" s="4"/>
+      <c r="AF82" s="4"/>
+      <c r="AG82" s="4"/>
+      <c r="AH82" s="4"/>
+      <c r="AI82" s="4"/>
+      <c r="AJ82" s="4">
+        <v>6</v>
+      </c>
+      <c r="AK82" s="4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="83" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A83" s="3">
+        <v>20100076</v>
+      </c>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="4">
+        <v>1</v>
+      </c>
+      <c r="K83" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="L83" s="4">
+        <v>1</v>
+      </c>
+      <c r="M83" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="N83" s="4">
+        <v>1</v>
+      </c>
+      <c r="O83" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P83" s="4"/>
+      <c r="Q83" s="4"/>
+      <c r="R83" s="4"/>
+      <c r="S83" s="4"/>
+      <c r="T83" s="4"/>
+      <c r="U83" s="4"/>
+      <c r="V83" s="4"/>
+      <c r="W83" s="4"/>
+      <c r="X83" s="4"/>
+      <c r="Y83" s="4"/>
+      <c r="Z83" s="4"/>
+      <c r="AA83" s="4"/>
+      <c r="AB83" s="4"/>
+      <c r="AC83" s="4"/>
+      <c r="AD83" s="4"/>
+      <c r="AE83" s="4"/>
+      <c r="AF83" s="4"/>
+      <c r="AG83" s="4"/>
+      <c r="AH83" s="4"/>
+      <c r="AI83" s="4"/>
+      <c r="AJ83" s="4">
+        <v>1</v>
+      </c>
+      <c r="AK83" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A84" s="3">
+        <v>20100083</v>
+      </c>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="4"/>
+      <c r="Q84" s="4"/>
+      <c r="R84" s="4"/>
+      <c r="S84" s="4"/>
+      <c r="T84" s="4"/>
+      <c r="U84" s="4"/>
+      <c r="V84" s="4"/>
+      <c r="W84" s="4"/>
+      <c r="X84" s="4"/>
+      <c r="Y84" s="4"/>
+      <c r="Z84" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA84" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="AB84" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC84" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="AD84" s="4"/>
+      <c r="AE84" s="4"/>
+      <c r="AF84" s="4"/>
+      <c r="AG84" s="4"/>
+      <c r="AH84" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI84" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="AJ84" s="4">
+        <v>1</v>
+      </c>
+      <c r="AK84" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="85" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A85" s="3">
+        <v>20100085</v>
+      </c>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
+      <c r="P85" s="4"/>
+      <c r="Q85" s="4"/>
+      <c r="R85" s="4"/>
+      <c r="S85" s="4"/>
+      <c r="T85" s="4">
+        <v>1</v>
+      </c>
+      <c r="U85" s="4">
+        <v>99</v>
+      </c>
+      <c r="V85" s="4">
+        <v>1</v>
+      </c>
+      <c r="W85" s="4">
+        <v>99</v>
+      </c>
+      <c r="X85" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y85" s="4">
+        <v>99</v>
+      </c>
+      <c r="Z85" s="4"/>
+      <c r="AA85" s="4"/>
+      <c r="AB85" s="4"/>
+      <c r="AC85" s="4"/>
+      <c r="AD85" s="4"/>
+      <c r="AE85" s="4"/>
+      <c r="AF85" s="4"/>
+      <c r="AG85" s="4"/>
+      <c r="AH85" s="4"/>
+      <c r="AI85" s="4"/>
+      <c r="AJ85" s="4">
+        <v>1</v>
+      </c>
+      <c r="AK85" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A86" s="3">
+        <v>20100090</v>
+      </c>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4">
+        <v>2</v>
+      </c>
+      <c r="G86" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H86" s="4">
+        <v>2</v>
+      </c>
+      <c r="I86" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4">
+        <v>2</v>
+      </c>
+      <c r="O86" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="4"/>
+      <c r="R86" s="4"/>
+      <c r="S86" s="4"/>
+      <c r="T86" s="4"/>
+      <c r="U86" s="4"/>
+      <c r="V86" s="4"/>
+      <c r="W86" s="4"/>
+      <c r="X86" s="4"/>
+      <c r="Y86" s="4"/>
+      <c r="Z86" s="4"/>
+      <c r="AA86" s="4"/>
+      <c r="AB86" s="4"/>
+      <c r="AC86" s="4"/>
+      <c r="AD86" s="4"/>
+      <c r="AE86" s="4"/>
+      <c r="AF86" s="4"/>
+      <c r="AG86" s="4"/>
+      <c r="AH86" s="4"/>
+      <c r="AI86" s="4"/>
+      <c r="AJ86" s="4">
+        <v>2</v>
+      </c>
+      <c r="AK86" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B87" s="4">
+        <v>2</v>
+      </c>
+      <c r="C87" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D87" s="4">
+        <v>2</v>
+      </c>
+      <c r="E87" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F87" s="4">
+        <v>2</v>
+      </c>
+      <c r="G87" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H87" s="4">
+        <v>2</v>
+      </c>
+      <c r="I87" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="J87" s="4">
+        <v>1</v>
+      </c>
+      <c r="K87" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="L87" s="4">
+        <v>1</v>
+      </c>
+      <c r="M87" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="N87" s="4">
+        <v>5</v>
+      </c>
+      <c r="O87" s="4">
+        <v>1247.25</v>
+      </c>
+      <c r="P87" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q87" s="4">
+        <v>199</v>
+      </c>
+      <c r="R87" s="4">
+        <v>6</v>
+      </c>
+      <c r="S87" s="4">
+        <v>199</v>
+      </c>
+      <c r="T87" s="4">
+        <v>1</v>
+      </c>
+      <c r="U87" s="4">
+        <v>99</v>
+      </c>
+      <c r="V87" s="4">
+        <v>1</v>
+      </c>
+      <c r="W87" s="4">
+        <v>99</v>
+      </c>
+      <c r="X87" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y87" s="4">
+        <v>298</v>
+      </c>
+      <c r="Z87" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA87" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="AB87" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC87" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="AD87" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE87" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="AF87" s="4">
+        <v>2</v>
+      </c>
+      <c r="AG87" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="AH87" s="4">
+        <v>3</v>
+      </c>
+      <c r="AI87" s="4">
+        <v>440.74</v>
+      </c>
+      <c r="AJ87" s="4">
+        <v>15</v>
+      </c>
+      <c r="AK87" s="4">
+        <v>1985.99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B91" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>8</v>
+      </c>
+      <c r="H92" t="s">
+        <v>10</v>
+      </c>
+      <c r="L92" t="s">
+        <v>13</v>
+      </c>
+      <c r="P92" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="93" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" t="s">
+        <v>15</v>
+      </c>
+      <c r="F93" t="s">
+        <v>7</v>
+      </c>
+      <c r="H93" t="s">
+        <v>15</v>
+      </c>
+      <c r="J93" t="s">
+        <v>7</v>
+      </c>
+      <c r="L93" t="s">
+        <v>12</v>
+      </c>
+      <c r="N93" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>29</v>
+      </c>
+      <c r="C94" t="s">
+        <v>19</v>
+      </c>
+      <c r="D94" t="s">
+        <v>29</v>
+      </c>
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
+        <v>29</v>
+      </c>
+      <c r="G94" t="s">
+        <v>19</v>
+      </c>
+      <c r="H94" t="s">
+        <v>29</v>
+      </c>
+      <c r="I94" t="s">
+        <v>19</v>
+      </c>
+      <c r="J94" t="s">
+        <v>29</v>
+      </c>
+      <c r="K94" t="s">
+        <v>19</v>
+      </c>
+      <c r="L94" t="s">
+        <v>29</v>
+      </c>
+      <c r="M94" t="s">
+        <v>19</v>
+      </c>
+      <c r="N94" t="s">
+        <v>29</v>
+      </c>
+      <c r="O94" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" t="s">
+        <v>9</v>
+      </c>
+      <c r="G95" t="s">
+        <v>9</v>
+      </c>
+      <c r="H95" t="s">
+        <v>16</v>
+      </c>
+      <c r="I95" t="s">
+        <v>16</v>
+      </c>
+      <c r="J95" t="s">
+        <v>11</v>
+      </c>
+      <c r="K95" t="s">
+        <v>11</v>
+      </c>
+      <c r="L95" t="s">
+        <v>14</v>
+      </c>
+      <c r="M95" t="s">
+        <v>14</v>
+      </c>
+      <c r="N95" t="s">
+        <v>9</v>
+      </c>
+      <c r="O95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A96" s="3">
+        <v>20100007</v>
+      </c>
+      <c r="B96" s="4">
+        <v>2</v>
+      </c>
+      <c r="C96" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
+      <c r="L96" s="4"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="4"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q96" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A97" s="3">
+        <v>20100017</v>
+      </c>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="4"/>
+      <c r="L97" s="4"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="4">
+        <v>2</v>
+      </c>
+      <c r="O97" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P97" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q97" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A98" s="3">
+        <v>20100070</v>
+      </c>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="4">
+        <v>6</v>
+      </c>
+      <c r="I98" s="4">
+        <v>199</v>
+      </c>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="4"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="4"/>
+      <c r="O98" s="4"/>
+      <c r="P98" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q98" s="4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A99" s="3">
+        <v>20100076</v>
+      </c>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4">
+        <v>1</v>
+      </c>
+      <c r="G99" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="4"/>
+      <c r="L99" s="4"/>
+      <c r="M99" s="4"/>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+      <c r="P99" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q99" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A100" s="3">
+        <v>20100083</v>
+      </c>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="4"/>
+      <c r="L100" s="4">
+        <v>1</v>
+      </c>
+      <c r="M100" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="N100" s="4"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q100" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A101" s="3">
+        <v>20100085</v>
+      </c>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="4"/>
+      <c r="J101" s="4">
+        <v>1</v>
+      </c>
+      <c r="K101" s="4">
+        <v>99</v>
+      </c>
+      <c r="L101" s="4"/>
+      <c r="M101" s="4"/>
+      <c r="N101" s="4"/>
+      <c r="O101" s="4"/>
+      <c r="P101" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q101" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A102" s="3">
+        <v>20100090</v>
+      </c>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4">
+        <v>2</v>
+      </c>
+      <c r="E102" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="4"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4"/>
+      <c r="L102" s="4"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="4"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q102" s="4">
+        <v>415.75</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A103" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103" s="4">
+        <v>2</v>
+      </c>
+      <c r="C103" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="D103" s="4">
+        <v>2</v>
+      </c>
+      <c r="E103" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="F103" s="4">
+        <v>1</v>
+      </c>
+      <c r="G103" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="H103" s="4">
+        <v>6</v>
+      </c>
+      <c r="I103" s="4">
+        <v>199</v>
+      </c>
+      <c r="J103" s="4">
+        <v>1</v>
+      </c>
+      <c r="K103" s="4">
+        <v>99</v>
+      </c>
+      <c r="L103" s="4">
+        <v>1</v>
+      </c>
+      <c r="M103" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="N103" s="4">
+        <v>2</v>
+      </c>
+      <c r="O103" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P103" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q103" s="4">
+        <v>1985.99</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B107" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>29</v>
+      </c>
+      <c r="L108" t="s">
+        <v>19</v>
+      </c>
+      <c r="V108" t="s">
+        <v>30</v>
+      </c>
+      <c r="W108" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>12</v>
+      </c>
+      <c r="D109" t="s">
+        <v>56</v>
+      </c>
+      <c r="E109" t="s">
+        <v>15</v>
+      </c>
+      <c r="H109" t="s">
+        <v>57</v>
+      </c>
+      <c r="I109" t="s">
+        <v>7</v>
+      </c>
+      <c r="K109" t="s">
+        <v>58</v>
+      </c>
+      <c r="L109" t="s">
+        <v>12</v>
+      </c>
+      <c r="N109" t="s">
+        <v>56</v>
+      </c>
+      <c r="O109" t="s">
+        <v>15</v>
+      </c>
+      <c r="R109" t="s">
+        <v>57</v>
+      </c>
+      <c r="S109" t="s">
+        <v>7</v>
+      </c>
+      <c r="U109" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B110" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110" t="s">
+        <v>13</v>
+      </c>
+      <c r="E110" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110" t="s">
+        <v>10</v>
+      </c>
+      <c r="G110" t="s">
+        <v>13</v>
+      </c>
+      <c r="I110" t="s">
+        <v>8</v>
+      </c>
+      <c r="J110" t="s">
+        <v>10</v>
+      </c>
+      <c r="L110" t="s">
+        <v>8</v>
+      </c>
+      <c r="M110" t="s">
+        <v>13</v>
+      </c>
+      <c r="O110" t="s">
+        <v>8</v>
+      </c>
+      <c r="P110" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>13</v>
+      </c>
+      <c r="S110" t="s">
+        <v>8</v>
+      </c>
+      <c r="T110" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A111" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" s="4">
+        <v>2</v>
+      </c>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4">
+        <v>2</v>
+      </c>
+      <c r="E111" s="4">
+        <v>2</v>
+      </c>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4">
+        <v>2</v>
+      </c>
+      <c r="H111" s="4">
+        <v>4</v>
+      </c>
+      <c r="I111" s="4">
+        <v>1</v>
+      </c>
+      <c r="J111" s="4"/>
+      <c r="K111" s="4">
+        <v>1</v>
+      </c>
+      <c r="L111" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="M111" s="4"/>
+      <c r="N111" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="O111" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P111" s="4"/>
+      <c r="Q111" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="R111" s="4">
+        <v>831.5</v>
+      </c>
+      <c r="S111" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="T111" s="4"/>
+      <c r="U111" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="V111" s="4">
+        <v>7</v>
+      </c>
+      <c r="W111" s="4">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A112" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4">
+        <v>1</v>
+      </c>
+      <c r="D112" s="4">
+        <v>1</v>
+      </c>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
+      <c r="J112" s="4"/>
+      <c r="K112" s="4"/>
+      <c r="L112" s="4"/>
+      <c r="M112" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="N112" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="O112" s="4"/>
+      <c r="P112" s="4"/>
+      <c r="Q112" s="4"/>
+      <c r="R112" s="4"/>
+      <c r="S112" s="4"/>
+      <c r="T112" s="4"/>
+      <c r="U112" s="4"/>
+      <c r="V112" s="4">
+        <v>1</v>
+      </c>
+      <c r="W112" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A113" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="4"/>
+      <c r="J113" s="4">
+        <v>1</v>
+      </c>
+      <c r="K113" s="4">
+        <v>1</v>
+      </c>
+      <c r="L113" s="4"/>
+      <c r="M113" s="4"/>
+      <c r="N113" s="4"/>
+      <c r="O113" s="4"/>
+      <c r="P113" s="4"/>
+      <c r="Q113" s="4"/>
+      <c r="R113" s="4"/>
+      <c r="S113" s="4"/>
+      <c r="T113" s="4">
+        <v>99</v>
+      </c>
+      <c r="U113" s="4">
+        <v>99</v>
+      </c>
+      <c r="V113" s="4">
+        <v>1</v>
+      </c>
+      <c r="W113" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A114" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4">
+        <v>6</v>
+      </c>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4">
+        <v>6</v>
+      </c>
+      <c r="I114" s="4"/>
+      <c r="J114" s="4"/>
+      <c r="K114" s="4"/>
+      <c r="L114" s="4"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="4"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4">
+        <v>199</v>
+      </c>
+      <c r="Q114" s="4"/>
+      <c r="R114" s="4">
+        <v>199</v>
+      </c>
+      <c r="S114" s="4"/>
+      <c r="T114" s="4"/>
+      <c r="U114" s="4"/>
+      <c r="V114" s="4">
+        <v>6</v>
+      </c>
+      <c r="W114" s="4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="115" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A115" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B115" s="4">
+        <v>2</v>
+      </c>
+      <c r="C115" s="4">
+        <v>1</v>
+      </c>
+      <c r="D115" s="4">
+        <v>3</v>
+      </c>
+      <c r="E115" s="4">
+        <v>2</v>
+      </c>
+      <c r="F115" s="4">
+        <v>6</v>
+      </c>
+      <c r="G115" s="4">
+        <v>2</v>
+      </c>
+      <c r="H115" s="4">
+        <v>10</v>
+      </c>
+      <c r="I115" s="4">
+        <v>1</v>
+      </c>
+      <c r="J115" s="4">
+        <v>1</v>
+      </c>
+      <c r="K115" s="4">
+        <v>2</v>
+      </c>
+      <c r="L115" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="M115" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="N115" s="4">
+        <v>440.74</v>
+      </c>
+      <c r="O115" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="P115" s="4">
+        <v>199</v>
+      </c>
+      <c r="Q115" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="R115" s="4">
+        <v>1030.5</v>
+      </c>
+      <c r="S115" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="T115" s="4">
+        <v>99</v>
+      </c>
+      <c r="U115" s="4">
+        <v>514.75</v>
+      </c>
+      <c r="V115" s="4">
+        <v>15</v>
+      </c>
+      <c r="W115" s="4">
+        <v>1985.99</v>
+      </c>
+    </row>
+    <row r="119" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B119" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>29</v>
+      </c>
+      <c r="I120" t="s">
+        <v>19</v>
+      </c>
+      <c r="P120" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="121" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>12</v>
+      </c>
+      <c r="D121" t="s">
+        <v>15</v>
+      </c>
+      <c r="G121" t="s">
+        <v>7</v>
+      </c>
+      <c r="I121" t="s">
+        <v>12</v>
+      </c>
+      <c r="K121" t="s">
+        <v>15</v>
+      </c>
+      <c r="N121" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B122" t="s">
+        <v>8</v>
+      </c>
+      <c r="C122" t="s">
+        <v>13</v>
+      </c>
+      <c r="D122" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" t="s">
+        <v>10</v>
+      </c>
+      <c r="F122" t="s">
+        <v>13</v>
+      </c>
+      <c r="G122" t="s">
+        <v>8</v>
+      </c>
+      <c r="H122" t="s">
+        <v>10</v>
+      </c>
+      <c r="I122" t="s">
+        <v>8</v>
+      </c>
+      <c r="J122" t="s">
+        <v>13</v>
+      </c>
+      <c r="K122" t="s">
+        <v>8</v>
+      </c>
+      <c r="L122" t="s">
+        <v>10</v>
+      </c>
+      <c r="M122" t="s">
+        <v>13</v>
+      </c>
+      <c r="N122" t="s">
+        <v>8</v>
+      </c>
+      <c r="O122" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A123" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B123" s="4">
+        <v>2</v>
+      </c>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4">
+        <v>2</v>
+      </c>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4">
+        <v>2</v>
+      </c>
+      <c r="G123" s="4">
+        <v>1</v>
+      </c>
+      <c r="H123" s="4"/>
+      <c r="I123" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="J123" s="4"/>
+      <c r="K123" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="L123" s="4"/>
+      <c r="M123" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="N123" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="O123" s="4"/>
+      <c r="P123" s="4">
+        <v>7</v>
+      </c>
+      <c r="Q123" s="4">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="124" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A124" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B124" s="4"/>
+      <c r="C124" s="4">
+        <v>1</v>
+      </c>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
+      <c r="H124" s="4"/>
+      <c r="I124" s="4"/>
+      <c r="J124" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="K124" s="4"/>
+      <c r="L124" s="4"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="4"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q124" s="4">
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="125" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="4">
+        <v>1</v>
+      </c>
+      <c r="I125" s="4"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="4"/>
+      <c r="L125" s="4"/>
+      <c r="M125" s="4"/>
+      <c r="N125" s="4"/>
+      <c r="O125" s="4">
+        <v>99</v>
+      </c>
+      <c r="P125" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q125" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="126" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A126" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4">
+        <v>6</v>
+      </c>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="4"/>
+      <c r="J126" s="4"/>
+      <c r="K126" s="4"/>
+      <c r="L126" s="4">
+        <v>199</v>
+      </c>
+      <c r="M126" s="4"/>
+      <c r="N126" s="4"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q126" s="4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A127" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B127" s="4">
+        <v>2</v>
+      </c>
+      <c r="C127" s="4">
+        <v>1</v>
+      </c>
+      <c r="D127" s="4">
+        <v>2</v>
+      </c>
+      <c r="E127" s="4">
+        <v>6</v>
+      </c>
+      <c r="F127" s="4">
+        <v>2</v>
+      </c>
+      <c r="G127" s="4">
+        <v>1</v>
+      </c>
+      <c r="H127" s="4">
+        <v>1</v>
+      </c>
+      <c r="I127" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="J127" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="K127" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="L127" s="4">
+        <v>199</v>
+      </c>
+      <c r="M127" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="N127" s="4">
+        <v>415.75</v>
+      </c>
+      <c r="O127" s="4">
+        <v>99</v>
+      </c>
+      <c r="P127" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q127" s="4">
         <v>1985.99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed pivot table address when there is only one column and no data fields.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
+++ b/EPPlusTest/Workbooks/PivotTableColumnFields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A5E68600-E034-46E6-98A3-7F4FACB72D61}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{836E78BB-5919-4AC8-B0E4-08000491D831}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9756" activeTab="6" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9756" xr2:uid="{73654E4E-98D9-4821-A4D4-63EE12428368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId8"/>
+    <pivotCache cacheId="3" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="62">
   <si>
     <t>Transaction</t>
   </si>
@@ -468,7 +468,1354 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E49A2269-CE94-412C-A399-800EF1C614AD}" name="Sheet1PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E27:E38" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{615E3895-2707-42E3-A785-8864A18E17EE}" name="MultipleDataFieldsPivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A10:W17" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="3">
+    <field x="3"/>
+    <field x="1"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="22">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i t="default" i="1">
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F81C657-F972-42B9-99B1-6B9FF9338C17}" name="MultipleDataFieldsPivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{275DFB84-4379-4C29-BE52-6943E478166B}" name="RowDataFieldsPivotTable5" cacheId="3" dataOnRows="1" dataPosition="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E37:F68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="31">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1CE963B4-85F1-470B-8720-5625E53AD926}" name="RowDataFieldsPivotTable1" cacheId="3" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1424B5F-181C-42B4-9454-6AAB7169E02E}" name="RowDataFieldsPivotTable4" cacheId="3" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A37:B48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BBD4942-F2DC-4306-B86C-66D12FC3A0F1}" name="RowDataFieldsPivotTable2" cacheId="3" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="H1:L31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="1"/>
+    <field x="3"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="29">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C74FC5-394B-4FAE-AEC0-2D1A8752CE1D}" name="RowDataFieldsPivotTable3" cacheId="3" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="O1:S52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="1"/>
+    <field x="3"/>
+    <field x="0"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="50">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="3"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D539B62D-4AC8-46E3-A8D4-1D8AFFC11145}" name="ColumnDataFieldsPivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A32:M39" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="3">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="12">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3118B986-EAC5-4497-83A8-B5E3225EEBB6}" name="ColumnDataFieldsPivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A11:I17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="-2"/>
+    <field x="2"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80E6C19D-DBE6-4B69-B9AA-DAA44B187BF6}" name="ColumnDataFieldsPivotTable10" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A119:Q127" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="3">
+    <field x="-2"/>
+    <field x="1"/>
+    <field x="2"/>
+  </colFields>
+  <colItems count="16">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96CD0C10-E2E0-4D68-8840-EEFB998C0C07}" name="Sheet1PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B12:R23" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -626,855 +1973,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{275DFB84-4379-4C29-BE52-6943E478166B}" name="RowDataFieldsPivotTable5" cacheId="10" dataOnRows="1" dataPosition="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E37:F68" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="2"/>
-    <field x="-2"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="31">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i t="default" i="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i t="default" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="default" i="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1CE963B4-85F1-470B-8720-5625E53AD926}" name="RowDataFieldsPivotTable1" cacheId="10" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="1"/>
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1424B5F-181C-42B4-9454-6AAB7169E02E}" name="RowDataFieldsPivotTable4" cacheId="10" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A37:B48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BBD4942-F2DC-4306-B86C-66D12FC3A0F1}" name="RowDataFieldsPivotTable2" cacheId="10" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="H1:L31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="1"/>
-    <field x="3"/>
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="29">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i t="default" i="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i t="default" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="default" i="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C74FC5-394B-4FAE-AEC0-2D1A8752CE1D}" name="RowDataFieldsPivotTable3" cacheId="10" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="O1:S52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" subtotalTop="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="4">
-    <field x="1"/>
-    <field x="3"/>
-    <field x="0"/>
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="50">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="3">
-      <x/>
-    </i>
-    <i r="3" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i t="default" r="1" i="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="4"/>
-    </i>
-    <i r="3">
-      <x/>
-    </i>
-    <i r="3" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i t="default" i="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="3">
-      <x/>
-    </i>
-    <i r="3" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="6"/>
-    </i>
-    <i r="3">
-      <x/>
-    </i>
-    <i r="3" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i t="default" r="1" i="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="3">
-      <x/>
-    </i>
-    <i r="3" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="3"/>
-    </i>
-    <i t="default" r="1" i="1">
-      <x v="3"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i t="default" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i r="3">
-      <x/>
-    </i>
-    <i r="3" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i t="default" r="1" i="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="5"/>
-    </i>
-    <i r="3">
-      <x/>
-    </i>
-    <i r="3" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1" i="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="default" i="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{80E6C19D-DBE6-4B69-B9AA-DAA44B187BF6}" name="ColumnDataFieldsPivotTable10" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A119:Q127" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="3">
-    <field x="-2"/>
-    <field x="1"/>
-    <field x="2"/>
-  </colFields>
-  <colItems count="16">
-    <i>
-      <x/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="2"/>
-    </i>
-    <i r="1" i="1">
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E5F8A30F-D02F-44BC-8036-0AB6A3D95E00}" name="ColumnDataFieldsPivotTable9" cacheId="10" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E5F8A30F-D02F-44BC-8036-0AB6A3D95E00}" name="ColumnDataFieldsPivotTable9" cacheId="3" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A107:W115" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1624,174 +2124,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8A4BBC34-425D-4477-AA03-0141BD5FAAD9}" name="ColumnDataFieldsPivotTable8" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A91:Q103" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="7">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="6"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="4">
-    <field x="2"/>
-    <field x="1"/>
-    <field x="-2"/>
-    <field x="3"/>
-  </colFields>
-  <colItems count="16">
-    <i>
-      <x/>
-      <x/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x v="1"/>
-      <x/>
-      <x v="3"/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x/>
-      <x v="2"/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{130E016C-4138-40D8-9FA8-D4183603FDA1}" name="ColumnDataFieldsPivotTable7" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{130E016C-4138-40D8-9FA8-D4183603FDA1}" name="ColumnDataFieldsPivotTable7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A75:AK87" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -2020,8 +2354,265 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43B65DE5-75DB-4432-AD36-D0F632525498}" name="ColumnDataFieldsPivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB40D58C-DD49-4477-9AD2-60BBD9C1D8DD}" name="ColumnDataFieldsPivotTable6" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A59:Q71" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="7">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="4">
+    <field x="2"/>
+    <field x="-2"/>
+    <field x="1"/>
+    <field x="3"/>
+  </colFields>
+  <colItems count="16">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="2" i="1">
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{66A9754B-81DC-4ED4-A80A-016D7E514761}" name="ColumnDataFieldsPivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:I7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="2"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{43B65DE5-75DB-4432-AD36-D0F632525498}" name="ColumnDataFieldsPivotTable5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A43:AK55" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -2249,521 +2840,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A26:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D539B62D-4AC8-46E3-A8D4-1D8AFFC11145}" name="ColumnDataFieldsPivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A32:M39" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="3">
-    <field x="2"/>
-    <field x="-2"/>
-    <field x="3"/>
-  </colFields>
-  <colItems count="12">
-    <i>
-      <x/>
-      <x/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x v="2"/>
-    </i>
-    <i r="2" i="1">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{66A9754B-81DC-4ED4-A80A-016D7E514761}" name="ColumnDataFieldsPivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:I7" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="2"/>
-    <field x="-2"/>
-  </colFields>
-  <colItems count="8">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{89F6948F-8455-4692-97DB-D9DBCCE61BCB}" name="ColumnDataFieldsPivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A21:S28" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="3">
-    <field x="2"/>
-    <field x="-2"/>
-    <field x="3"/>
-  </colFields>
-  <colItems count="18">
-    <i>
-      <x/>
-      <x/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i t="default" i="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x v="2"/>
-    </i>
-    <i r="2" i="1">
-      <x v="3"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i t="default" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="default" i="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3118B986-EAC5-4497-83A8-B5E3225EEBB6}" name="ColumnDataFieldsPivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A11:I17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="-2"/>
-    <field x="2"/>
-  </colFields>
-  <colItems count="8">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1" i="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB40D58C-DD49-4477-9AD2-60BBD9C1D8DD}" name="ColumnDataFieldsPivotTable6" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A59:Q71" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable25.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8A4BBC34-425D-4477-AA03-0141BD5FAAD9}" name="ColumnDataFieldsPivotTable8" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A91:Q103" firstHeaderRow="1" firstDataRow="5" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
       <items count="7">
@@ -2833,8 +2912,8 @@
   </rowItems>
   <colFields count="4">
     <field x="2"/>
+    <field x="1"/>
     <field x="-2"/>
-    <field x="1"/>
     <field x="3"/>
   </colFields>
   <colItems count="16">
@@ -2844,60 +2923,61 @@
       <x/>
       <x/>
     </i>
-    <i r="2">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2">
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x/>
-      <x/>
-    </i>
     <i r="2" i="1">
       <x v="1"/>
       <x/>
     </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+      <x/>
+    </i>
     <i r="2" i="1">
-      <x v="2"/>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="1"/>
+      <x/>
       <x v="3"/>
     </i>
-    <i r="2">
-      <x v="2"/>
-      <x v="2"/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
+    <i r="2" i="1">
       <x v="1"/>
       <x v="3"/>
     </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+      <x v="2"/>
+    </i>
     <i r="2" i="1">
-      <x v="2"/>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+      <x/>
     </i>
     <i r="2" i="1">
       <x v="1"/>
@@ -2926,13 +3006,20 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{89F6948F-8455-4692-97DB-D9DBCCE61BCB}" name="ColumnDataFieldsPivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A21:S28" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
@@ -2940,7 +3027,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisCol" showAll="0">
       <items count="5">
         <item x="0"/>
         <item x="2"/>
@@ -2949,48 +3036,100 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField numFmtId="8" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
   </pivotFields>
-  <rowFields count="2">
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="3">
     <field x="2"/>
+    <field x="-2"/>
     <field x="3"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
+  </colFields>
+  <colItems count="18">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="default" i="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i r="2">
       <x v="3"/>
     </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x v="2"/>
+    </i>
+    <i r="2" i="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="default" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2" i="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="default" i="1">
+      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
     </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
+    <i t="grand" i="1">
+      <x/>
+    </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  <dataFields count="2">
+    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Wholesale Price" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3004,8 +3143,59 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B348EB60-7EB8-41C3-924D-831797F7D06A}" name="Sheet1PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B27:B31" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2863EB01-E6CF-4B74-B171-2729E8FCA1EA}" name="RowItemsPivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3059,7 +3249,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA08530B-CFB9-46FF-92C2-2B99FF0DE8A8}" name="RowItemsPivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L1:M17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3166,7 +3356,161 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BB19D0AE-E5EA-48C1-95D4-31B1841FF10A}" name="RowItemsPivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A26:B35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{630F8736-78FD-4115-B74D-728639351C47}" name="RowItemsPivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F1:G10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="8" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="8" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B056D19-F4FF-46AF-8B83-8B1081758FA1}" name="NoSubtotalsPivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:I13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -3286,8 +3630,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0326097-9F86-483D-9D84-951795ECF9D4}" name="GrandTotalsPivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:L8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -3383,219 +3727,6 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{615E3895-2707-42E3-A785-8864A18E17EE}" name="MultipleDataFieldsPivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A10:W17" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="3">
-    <field x="3"/>
-    <field x="1"/>
-    <field x="-2"/>
-  </colFields>
-  <colItems count="22">
-    <i>
-      <x/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i t="default" i="1">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i t="default" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i t="default" i="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2" i="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="3"/>
-    </i>
-    <i t="default" i="1">
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F81C657-F972-42B9-99B1-6B9FF9338C17}" name="MultipleDataFieldsPivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="8" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="8" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Units Sold" fld="5" baseField="0" baseItem="0"/>
     <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -3907,19 +4038,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86234C7-1633-473D-AAFD-744E7802C65D}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -4462,6 +4593,81 @@
       </c>
       <c r="R23" s="4">
         <v>1985.99</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="E32" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E38" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -7116,7 +7322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE2431C-D3CF-40A9-83CD-D04719B9BC4E}">
   <dimension ref="A1:AK127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>

</xml_diff>